<commit_message>
Ajout commande Mouser à l'excel de commande
</commit_message>
<xml_diff>
--- a/EL_Electrical/Commande-janvier.xlsx
+++ b/EL_Electrical/Commande-janvier.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lecoc\Desktop\EPSA\Ressource 2020\EL_Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobau\Documents\EPSA\Ressources2020\EL_Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RS Component" sheetId="1" r:id="rId1"/>
     <sheet name="Farnell" sheetId="2" r:id="rId2"/>
+    <sheet name="Mouser" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="292">
   <si>
     <t>Description</t>
   </si>
@@ -762,18 +763,178 @@
   <si>
     <t>TE Connectivity</t>
   </si>
+  <si>
+    <t>Référence</t>
+  </si>
+  <si>
+    <t>Dénomination</t>
+  </si>
+  <si>
+    <t>Description (si nécessaire)</t>
+  </si>
+  <si>
+    <t>Prix TTC</t>
+  </si>
+  <si>
+    <t>Réduction</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Prix total HT</t>
+  </si>
+  <si>
+    <t>Prix total TTC</t>
+  </si>
+  <si>
+    <t>576-PDM71001ZXM</t>
+  </si>
+  <si>
+    <t>829-12010300</t>
+  </si>
+  <si>
+    <t>Cavity plug</t>
+  </si>
+  <si>
+    <t>829-12084201</t>
+  </si>
+  <si>
+    <t>Connecteur 0.35-0.50 mm2</t>
+  </si>
+  <si>
+    <t>20-22AWG</t>
+  </si>
+  <si>
+    <t>829-12077411</t>
+  </si>
+  <si>
+    <t>Connecteur 0.50-1.00 mm2</t>
+  </si>
+  <si>
+    <t>17-20AWG</t>
+  </si>
+  <si>
+    <t>829-15363933</t>
+  </si>
+  <si>
+    <t>Connecteur 1.00-2.00 mm2</t>
+  </si>
+  <si>
+    <t>14-17AWG</t>
+  </si>
+  <si>
+    <t>829-12129493</t>
+  </si>
+  <si>
+    <t>Connecteur 2.00-3.00 mm2</t>
+  </si>
+  <si>
+    <t>12-14AWG</t>
+  </si>
+  <si>
+    <t>829-12077413</t>
+  </si>
+  <si>
+    <t>Connecteur 5.00 mm2</t>
+  </si>
+  <si>
+    <t>8AWG</t>
+  </si>
+  <si>
+    <t>829-15324983</t>
+  </si>
+  <si>
+    <t>CABLE SEAL DARK RED</t>
+  </si>
+  <si>
+    <t>829-15324985</t>
+  </si>
+  <si>
+    <t>CABLE SEAL PURPLE</t>
+  </si>
+  <si>
+    <t>829-15324982</t>
+  </si>
+  <si>
+    <t>CBL SEAL GREEN</t>
+  </si>
+  <si>
+    <t>829-15324980</t>
+  </si>
+  <si>
+    <t>CBL SEAL GRAY</t>
+  </si>
+  <si>
+    <t>829-15324981</t>
+  </si>
+  <si>
+    <t>CBL SEAL BLUE</t>
+  </si>
+  <si>
+    <t>893-3011ASR112VDC</t>
+  </si>
+  <si>
+    <t>Relais</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>504-BP/FB6-ATM</t>
+  </si>
+  <si>
+    <t>Boîte à fusibles arrière</t>
+  </si>
+  <si>
+    <t>787-3852</t>
+  </si>
+  <si>
+    <t>facade DB-9</t>
+  </si>
+  <si>
+    <t>Connecteur Sub-D, 9 Contacts, Femelle, Montage sur câble, Standard</t>
+  </si>
+  <si>
+    <t>MHDB9SS</t>
+  </si>
+  <si>
+    <t>MH Connector</t>
+  </si>
+  <si>
+    <t>https://fr.rs-online.com/web/p/connecteurs-sub-d-a-souder/7873852/?relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E2828282872737C5253295B205D3F293F285C647B337D5B5C2D5C735D3F5C647B332C347D5B705061415D3F29297C283235285C647B387D7C5C647B317D5C2D5C647B377D2929292426706F3D3126736E3D592673723D2673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3738372D33383532267374613D3738373338353226&amp;searchHistory=%7B"enabled"%3Atrue%7D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+  <si>
+    <t>523-17HD015PAM030</t>
+  </si>
+  <si>
+    <t>Connecteur D sub 15 HD</t>
+  </si>
+  <si>
+    <t>Back shell sub D 15</t>
+  </si>
+  <si>
+    <t>981-009-130R121</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
-    <numFmt numFmtId="171" formatCode="#,##0.000\ &quot;€&quot;"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0000\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000\ &quot;€&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,16 +987,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -927,6 +1109,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -934,7 +1174,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -991,20 +1231,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1016,7 +1256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,11 +1272,54 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1045,7 +1328,24 @@
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1071,8 +1371,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="#,##0.0000\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1089,24 +1388,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0000\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1271,6 +1554,23 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1411,17 +1711,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:H27"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Composant/Pièce" dataDxfId="18"/>
-    <tableColumn id="2" name="Description" dataDxfId="17"/>
-    <tableColumn id="3" name="Code commande" dataDxfId="16"/>
-    <tableColumn id="4" name="Fabricant" dataDxfId="15"/>
-    <tableColumn id="5" name="Réf. Fabricant" dataDxfId="14"/>
-    <tableColumn id="6" name="Qté unitaire/mètre" dataDxfId="13"/>
-    <tableColumn id="7" name="Prix unitaire HT" dataDxfId="12"/>
-    <tableColumn id="8" name="Lien" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I27" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:I27"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Composant/Pièce" dataDxfId="19"/>
+    <tableColumn id="2" name="Description" dataDxfId="18"/>
+    <tableColumn id="3" name="Code commande" dataDxfId="17"/>
+    <tableColumn id="4" name="Fabricant" dataDxfId="16"/>
+    <tableColumn id="5" name="Réf. Fabricant" dataDxfId="15"/>
+    <tableColumn id="6" name="Qté unitaire/mètre" dataDxfId="14"/>
+    <tableColumn id="7" name="Prix unitaire HT" dataDxfId="13"/>
+    <tableColumn id="8" name="Lien" dataDxfId="12"/>
+    <tableColumn id="9" name="Colonne1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1437,9 +1738,9 @@
     <tableColumn id="4" name="Fabricant" dataDxfId="6" dataCellStyle="Excel Built-in Normal"/>
     <tableColumn id="5" name="Réf. Fabricant" dataDxfId="5" dataCellStyle="Excel Built-in Normal"/>
     <tableColumn id="6" name="Qté unitaire/mètre" dataDxfId="4" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="7" name="Prix unitaire HT" dataDxfId="1" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="8" name="Lien" dataDxfId="3" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="11" name="Prix HT" dataDxfId="0" dataCellStyle="Excel Built-in Normal">
+    <tableColumn id="7" name="Prix unitaire HT" dataDxfId="3" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="8" name="Lien" dataDxfId="2" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="11" name="Prix HT" dataDxfId="1" dataCellStyle="Excel Built-in Normal">
       <calculatedColumnFormula>Tableau13[[#This Row],[Qté unitaire/mètre]]*Tableau13[[#This Row],[Prix unitaire HT]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1713,23 +2014,23 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="100.77734375" customWidth="1"/>
-    <col min="9" max="16" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+    <col min="9" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1754,8 +2055,11 @@
       <c r="H1" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="I1" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>115</v>
       </c>
@@ -1778,7 +2082,7 @@
       <c r="H2" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1787,7 +2091,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="86.4">
+    <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>160</v>
       </c>
@@ -1812,7 +2116,7 @@
       <c r="H3" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1821,7 +2125,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="43.2">
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>114</v>
       </c>
@@ -1834,7 +2138,7 @@
       <c r="H4" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1843,7 +2147,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="57.6">
+    <row r="5" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>124</v>
       </c>
@@ -1866,7 +2170,7 @@
       <c r="H5" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1875,16 +2179,34 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1.45</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1893,7 +2215,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1902,7 +2224,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="36"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1911,7 +2233,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1920,7 +2242,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="36"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1929,7 +2251,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1938,7 +2260,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="36"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1947,7 +2269,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1956,7 +2278,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="36"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1965,7 +2287,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1974,7 +2296,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="36"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1983,7 +2305,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1992,7 +2314,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="36"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -2001,7 +2323,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2010,7 +2332,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="36"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2019,7 +2341,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2028,7 +2350,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="36"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2037,7 +2359,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2046,7 +2368,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="36"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2055,7 +2377,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2064,7 +2386,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="36"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2073,7 +2395,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2082,7 +2404,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="36"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2091,7 +2413,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2100,7 +2422,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="36"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="2"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2109,7 +2431,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2118,7 +2440,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="36"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2127,7 +2449,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2136,7 +2458,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="36"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2145,7 +2467,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2154,7 +2476,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="36"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
+      <c r="I21" s="2"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2163,7 +2485,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2172,7 +2494,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="36"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2181,7 +2503,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2190,7 +2512,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="36"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="2"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2199,7 +2521,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2208,7 +2530,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="36"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2217,7 +2539,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2226,7 +2548,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="36"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="1"/>
+      <c r="I25" s="2"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2235,7 +2557,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2244,7 +2566,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="36"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
+      <c r="I26" s="2"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2253,7 +2575,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2262,7 +2584,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="3"/>
       <c r="H27" s="18"/>
-      <c r="I27" s="1"/>
+      <c r="I27" s="18"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2276,6 +2598,7 @@
     <hyperlink ref="H4" r:id="rId1"/>
     <hyperlink ref="D5" r:id="rId2"/>
     <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="H6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2288,23 +2611,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2333,7 +2656,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="72">
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -2363,7 +2686,7 @@
         <v>0.114</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -2393,7 +2716,7 @@
         <v>0.114</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="72">
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -2423,7 +2746,7 @@
         <v>0.19199999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="72">
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -2453,7 +2776,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="72">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -2483,7 +2806,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="158.4">
+    <row r="7" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -2513,7 +2836,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="158.4">
+    <row r="8" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -2543,7 +2866,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="158.4">
+    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -2573,7 +2896,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="144">
+    <row r="10" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -2603,7 +2926,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="158.4">
+    <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
@@ -2633,7 +2956,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="100.8">
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
@@ -2663,7 +2986,7 @@
         <v>1.5629999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="86.4">
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
@@ -2693,7 +3016,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="86.4">
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
@@ -2723,7 +3046,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="100.8">
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
@@ -2753,7 +3076,7 @@
         <v>0.59699999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="100.8">
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>51</v>
       </c>
@@ -2783,7 +3106,7 @@
         <v>1.6900000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="86.4">
+    <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -2813,7 +3136,7 @@
         <v>5.34</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="100.8">
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>58</v>
       </c>
@@ -2843,7 +3166,7 @@
         <v>1.3900000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="86.4">
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>61</v>
       </c>
@@ -2873,7 +3196,7 @@
         <v>7.47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="72">
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>64</v>
       </c>
@@ -2903,7 +3226,7 @@
         <v>3.0149999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="72">
+    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>67</v>
       </c>
@@ -2933,7 +3256,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="72">
+    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>71</v>
       </c>
@@ -2963,7 +3286,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="144">
+    <row r="23" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
@@ -2993,7 +3316,7 @@
         <v>3.5100000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72">
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>78</v>
       </c>
@@ -3023,7 +3346,7 @@
         <v>1.4835</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="158.4">
+    <row r="25" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>81</v>
       </c>
@@ -3053,7 +3376,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="158.4">
+    <row r="26" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>84</v>
       </c>
@@ -3083,7 +3406,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="144">
+    <row r="27" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>87</v>
       </c>
@@ -3113,7 +3436,7 @@
         <v>1.905</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="158.4">
+    <row r="28" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>90</v>
       </c>
@@ -3143,7 +3466,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="144">
+    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>93</v>
       </c>
@@ -3173,7 +3496,7 @@
         <v>2.0100000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="144">
+    <row r="30" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>96</v>
       </c>
@@ -3203,7 +3526,7 @@
         <v>1.1600000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="129.6">
+    <row r="31" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>99</v>
       </c>
@@ -3233,7 +3556,7 @@
         <v>3.9550000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="129.6">
+    <row r="32" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>102</v>
       </c>
@@ -3263,7 +3586,7 @@
         <v>1.4749999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="144">
+    <row r="33" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>105</v>
       </c>
@@ -3293,7 +3616,7 @@
         <v>33.08</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="115.2">
+    <row r="34" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>106</v>
       </c>
@@ -3323,7 +3646,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="86.4">
+    <row r="35" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>110</v>
       </c>
@@ -3353,7 +3676,7 @@
         <v>2.3250000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="100.8">
+    <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>116</v>
       </c>
@@ -3383,7 +3706,7 @@
         <v>5.8019999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="57.6">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>120</v>
       </c>
@@ -3413,7 +3736,7 @@
         <v>5.226</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="86.4">
+    <row r="38" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>128</v>
       </c>
@@ -3443,7 +3766,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="72">
+    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>131</v>
       </c>
@@ -3473,7 +3796,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="86.4">
+    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>135</v>
       </c>
@@ -3503,7 +3826,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="100.8">
+    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>138</v>
       </c>
@@ -3533,7 +3856,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="129.6">
+    <row r="42" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>140</v>
       </c>
@@ -3563,7 +3886,7 @@
         <v>6.38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="129.6">
+    <row r="43" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>143</v>
       </c>
@@ -3589,7 +3912,7 @@
         <v>27.950000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="100.8">
+    <row r="44" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>144</v>
       </c>
@@ -3619,7 +3942,7 @@
         <v>13.45</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="100.8">
+    <row r="45" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>148</v>
       </c>
@@ -3649,7 +3972,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="100.8">
+    <row r="46" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>152</v>
       </c>
@@ -3679,7 +4002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="144">
+    <row r="47" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>155</v>
       </c>
@@ -3705,7 +4028,7 @@
         <v>24.94</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="144">
+    <row r="48" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>156</v>
       </c>
@@ -3735,7 +4058,7 @@
         <v>34.76</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="86.4">
+    <row r="49" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>226</v>
       </c>
@@ -3765,7 +4088,7 @@
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="129.6">
+    <row r="50" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>226</v>
       </c>
@@ -3840,4 +4163,546 @@
     <tablePart r:id="rId38"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="44">
+        <v>21.23</v>
+      </c>
+      <c r="E2" s="44">
+        <f>1.2*D2</f>
+        <v>25.475999999999999</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="42">
+        <v>1</v>
+      </c>
+      <c r="H2" s="44">
+        <f>D2*G2</f>
+        <v>21.23</v>
+      </c>
+      <c r="I2" s="44">
+        <f>E2*G2</f>
+        <v>25.475999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="44">
+        <v>0.19</v>
+      </c>
+      <c r="E3" s="44">
+        <f t="shared" ref="E3:E17" si="0">1.2*D3</f>
+        <v>0.22799999999999998</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="42">
+        <v>30</v>
+      </c>
+      <c r="H3" s="44">
+        <f t="shared" ref="H3:H15" si="1">D3*G3</f>
+        <v>5.7</v>
+      </c>
+      <c r="I3" s="44">
+        <f t="shared" ref="I3:I15" si="2">E3*G3</f>
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="44">
+        <v>0.22</v>
+      </c>
+      <c r="E4" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F4" s="43"/>
+      <c r="G4" s="42">
+        <v>25</v>
+      </c>
+      <c r="H4" s="44">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="I4" s="44">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0.39</v>
+      </c>
+      <c r="E5" s="44">
+        <f t="shared" si="0"/>
+        <v>0.46799999999999997</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="42">
+        <v>25</v>
+      </c>
+      <c r="H5" s="44">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="I5" s="44">
+        <f t="shared" si="2"/>
+        <v>11.7</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D6" s="44">
+        <v>0.22</v>
+      </c>
+      <c r="E6" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="42">
+        <v>25</v>
+      </c>
+      <c r="H6" s="44">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="I6" s="44">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="44">
+        <v>0.24</v>
+      </c>
+      <c r="E7" s="44">
+        <f t="shared" si="0"/>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="F7" s="43"/>
+      <c r="G7" s="42">
+        <v>25</v>
+      </c>
+      <c r="H7" s="44">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="44">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0.23</v>
+      </c>
+      <c r="E8" s="44">
+        <f t="shared" si="0"/>
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="F8" s="43"/>
+      <c r="G8" s="42">
+        <v>25</v>
+      </c>
+      <c r="H8" s="44">
+        <f t="shared" si="1"/>
+        <v>5.75</v>
+      </c>
+      <c r="I8" s="44">
+        <f t="shared" si="2"/>
+        <v>6.9</v>
+      </c>
+      <c r="J8" s="45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44">
+        <v>0.13</v>
+      </c>
+      <c r="E9" s="44">
+        <f t="shared" si="0"/>
+        <v>0.156</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="42">
+        <v>25</v>
+      </c>
+      <c r="H9" s="44">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="I9" s="44">
+        <f t="shared" si="2"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="E10" s="44">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="42">
+        <v>25</v>
+      </c>
+      <c r="H10" s="44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I10" s="44">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="44">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="F11" s="43"/>
+      <c r="G11" s="42">
+        <v>25</v>
+      </c>
+      <c r="H11" s="44">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I11" s="44">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="44">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="42">
+        <v>25</v>
+      </c>
+      <c r="H12" s="44">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I12" s="44">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="44">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="42">
+        <v>25</v>
+      </c>
+      <c r="H13" s="44">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I13" s="44">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" s="44">
+        <v>3.19</v>
+      </c>
+      <c r="E14" s="44">
+        <f t="shared" si="0"/>
+        <v>3.8279999999999998</v>
+      </c>
+      <c r="F14" s="43"/>
+      <c r="G14" s="42">
+        <v>4</v>
+      </c>
+      <c r="H14" s="44">
+        <f t="shared" si="1"/>
+        <v>12.76</v>
+      </c>
+      <c r="I14" s="44">
+        <f t="shared" si="2"/>
+        <v>15.311999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="D15" s="44">
+        <v>46.31</v>
+      </c>
+      <c r="E15" s="44">
+        <f t="shared" si="0"/>
+        <v>55.572000000000003</v>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="42">
+        <v>1</v>
+      </c>
+      <c r="H15" s="44">
+        <f t="shared" si="1"/>
+        <v>46.31</v>
+      </c>
+      <c r="I15" s="44">
+        <f t="shared" si="2"/>
+        <v>55.572000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="44">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E16" s="44">
+        <f t="shared" si="0"/>
+        <v>5.28</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="42">
+        <v>1</v>
+      </c>
+      <c r="H16" s="44">
+        <f t="shared" ref="H16:H17" si="3">D16*G16</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I16" s="44">
+        <f t="shared" ref="I16:I17" si="4">E16*G16</f>
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="44">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E17" s="44">
+        <f t="shared" si="0"/>
+        <v>5.8319999999999999</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="42">
+        <v>1</v>
+      </c>
+      <c r="H17" s="44">
+        <f t="shared" si="3"/>
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="I17" s="44">
+        <f t="shared" si="4"/>
+        <v>5.8319999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48">
+        <f>SUM(I2:I17)</f>
+        <v>168.61199999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D19:H20"/>
+    <mergeCell ref="I19:I20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>